<commit_message>
Did a sanity test of initializing a BRAM content with COE file.
</commit_message>
<xml_diff>
--- a/FPGA/bram/doc/BRAM.xlsx
+++ b/FPGA/bram/doc/BRAM.xlsx
@@ -349,778 +349,1290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A128"/>
+  <dimension ref="A1:B128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="str">
+        <f>DEC2HEX(A1, 4)</f>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="str">
+        <f t="shared" ref="B2:B65" si="0">DEC2HEX(A2, 4)</f>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>MOD(A1+A2, 2^16)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
+        <f t="shared" si="0"/>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A67" si="0">MOD(A2+A3, 2^16)</f>
+        <f t="shared" ref="A4:A67" si="1">MOD(A2+A3, 2^16)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>0002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>0003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>0005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>0008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>000D</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>0015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>0022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>0037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>0059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>144</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>0090</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>233</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>00E9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>377</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>0179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>610</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>0262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>987</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>03DB</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1597</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>063D</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2584</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>0A18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4181</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6765</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>1A6D</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10946</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>2AC2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17711</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>452F</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28657</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>6FF1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46368</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>B520</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9489</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55857</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>DA31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>65346</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>FF42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55667</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>D973</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>55477</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>D8B5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45608</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>B228</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35549</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>8ADD</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15621</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>3D05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51170</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>C7E2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1255</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>04E7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52425</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>CCC9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>53680</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>D1B0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40569</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>9E79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28713</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>7029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3746</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>0EA2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32459</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>7ECB</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36205</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>8D6D</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3128</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>0C38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39333</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>99A5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42461</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>A5DD</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16258</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>3F82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58719</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>E55F</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9441</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>24E1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2624</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>0A40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12065</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>2F21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14689</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26754</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>6882</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41443</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>A1E3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2661</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>0A65</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44104</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>AC48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46765</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>B6AD</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25333</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>62F5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6562</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>19A2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31895</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>7C97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38457</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>9639</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4816</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>12D0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43273</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>A909</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>48089</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>BBD9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25826</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>64E2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8379</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>20BB</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34205</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="str">
+        <f t="shared" ref="B66:B128" si="2">DEC2HEX(A66, 4)</f>
+        <v>859D</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>42584</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="str">
+        <f t="shared" si="2"/>
+        <v>A658</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" ref="A68:A128" si="1">MOD(A66+A67, 2^16)</f>
+        <f t="shared" ref="A68:A128" si="3">MOD(A66+A67, 2^16)</f>
         <v>11253</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="str">
+        <f t="shared" si="2"/>
+        <v>2BF5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53837</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="str">
+        <f t="shared" si="2"/>
+        <v>D24D</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>65090</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="str">
+        <f t="shared" si="2"/>
+        <v>FE42</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53391</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="str">
+        <f t="shared" si="2"/>
+        <v>D08F</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52945</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="str">
+        <f t="shared" si="2"/>
+        <v>CED1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40800</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="str">
+        <f t="shared" si="2"/>
+        <v>9F60</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>28209</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="str">
+        <f t="shared" si="2"/>
+        <v>6E31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>3473</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="str">
+        <f t="shared" si="2"/>
+        <v>0D91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31682</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="str">
+        <f t="shared" si="2"/>
+        <v>7BC2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35155</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="str">
+        <f t="shared" si="2"/>
+        <v>8953</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1301</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="str">
+        <f t="shared" si="2"/>
+        <v>0515</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>36456</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="str">
+        <f t="shared" si="2"/>
+        <v>8E68</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>37757</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="str">
+        <f t="shared" si="2"/>
+        <v>937D</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8677</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="str">
+        <f t="shared" si="2"/>
+        <v>21E5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>46434</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="str">
+        <f t="shared" si="2"/>
+        <v>B562</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>55111</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="str">
+        <f t="shared" si="2"/>
+        <v>D747</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>36009</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="str">
+        <f t="shared" si="2"/>
+        <v>8CA9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25584</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="str">
+        <f t="shared" si="2"/>
+        <v>63F0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>61593</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="str">
+        <f t="shared" si="2"/>
+        <v>F099</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>21641</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="str">
+        <f t="shared" si="2"/>
+        <v>5489</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17698</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="str">
+        <f t="shared" si="2"/>
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39339</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="str">
+        <f t="shared" si="2"/>
+        <v>99AB</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>57037</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" t="str">
+        <f t="shared" si="2"/>
+        <v>DECD</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30840</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B91" t="str">
+        <f t="shared" si="2"/>
+        <v>7878</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>22341</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B92" t="str">
+        <f t="shared" si="2"/>
+        <v>5745</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>53181</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B93" t="str">
+        <f t="shared" si="2"/>
+        <v>CFBD</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9986</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B94" t="str">
+        <f t="shared" si="2"/>
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>63167</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B95" t="str">
+        <f t="shared" si="2"/>
+        <v>F6BF</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7617</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" t="str">
+        <f t="shared" si="2"/>
+        <v>1DC1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5248</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" t="str">
+        <f t="shared" si="2"/>
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12865</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" t="str">
+        <f t="shared" si="2"/>
+        <v>3241</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18113</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" t="str">
+        <f t="shared" si="2"/>
+        <v>46C1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30978</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" t="str">
+        <f t="shared" si="2"/>
+        <v>7902</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>49091</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" t="str">
+        <f t="shared" si="2"/>
+        <v>BFC3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>14533</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" t="str">
+        <f t="shared" si="2"/>
+        <v>38C5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>63624</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" t="str">
+        <f t="shared" si="2"/>
+        <v>F888</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12621</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" t="str">
+        <f t="shared" si="2"/>
+        <v>314D</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10709</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" t="str">
+        <f t="shared" si="2"/>
+        <v>29D5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>23330</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" t="str">
+        <f t="shared" si="2"/>
+        <v>5B22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34039</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" t="str">
+        <f t="shared" si="2"/>
+        <v>84F7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>57369</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" t="str">
+        <f t="shared" si="2"/>
+        <v>E019</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25872</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" t="str">
+        <f t="shared" si="2"/>
+        <v>6510</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>17705</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" t="str">
+        <f t="shared" si="2"/>
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43577</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" t="str">
+        <f t="shared" si="2"/>
+        <v>AA39</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>61282</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" t="str">
+        <f t="shared" si="2"/>
+        <v>EF62</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39323</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" t="str">
+        <f t="shared" si="2"/>
+        <v>999B</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35069</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" t="str">
+        <f t="shared" si="2"/>
+        <v>88FD</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8856</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" t="str">
+        <f t="shared" si="2"/>
+        <v>2298</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43925</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" t="str">
+        <f t="shared" si="2"/>
+        <v>AB95</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52781</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" t="str">
+        <f t="shared" si="2"/>
+        <v>CE2D</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>31170</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" t="str">
+        <f t="shared" si="2"/>
+        <v>79C2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>18415</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119" t="str">
+        <f t="shared" si="2"/>
+        <v>47EF</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>49585</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120" t="str">
+        <f t="shared" si="2"/>
+        <v>C1B1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2464</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121" t="str">
+        <f t="shared" si="2"/>
+        <v>09A0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52049</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122" t="str">
+        <f t="shared" si="2"/>
+        <v>CB51</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>54513</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123" t="str">
+        <f t="shared" si="2"/>
+        <v>D4F1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>41026</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124" t="str">
+        <f t="shared" si="2"/>
+        <v>A042</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>30003</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125" t="str">
+        <f t="shared" si="2"/>
+        <v>7533</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5493</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126" t="str">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35496</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127" t="str">
+        <f t="shared" si="2"/>
+        <v>8AA8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>40989</v>
+      </c>
+      <c r="B128" t="str">
+        <f t="shared" si="2"/>
+        <v>A01D</v>
       </c>
     </row>
   </sheetData>

</xml_diff>